<commit_message>
UPDATED PREPROCESS EDF -> FIF API, TESTING, ELECTRODE OBJECT
Created new electrode object, not in use yet. Has functionality for regex on

Added more tests to reach 83% coverage.

Updated preprocess API for going from EDF file + clinical metadata + electrode layout sheet
to a .fif + .json file.

Squashed commit of the following:

commit 98b2945bf4a4d8ae95303aa5c8bc00fc0262e17d
Author: Adam Li <adam2392@gmail.com>
Date:   Sun Oct 6 22:37:47 2019 -0400

    Adding new test electrode layout data. Adding better functionality for loading and also made an API test to preprocess EDF files, with an accompanying patient clinical data sheet, and electrode layout sheet.
</commit_message>
<xml_diff>
--- a/data/clinical_examples/test_clinicaldata.xlsx
+++ b/data/clinical_examples/test_clinicaldata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam2392/Documents/eegio/data/clinical_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D87417D-D396-8547-A58E-DDA903F803A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7DBBBF-3CD4-4E48-BCB7-314C04A94B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11260" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{3613ACA9-70DC-9341-9578-D2DE191679B9}"/>
+    <workbookView xWindow="1660" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{3613ACA9-70DC-9341-9578-D2DE191679B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>patient_id</t>
   </si>
@@ -57,9 +57,6 @@
     <t>imaging_outcome_notes</t>
   </si>
   <si>
-    <t>bad_channels</t>
-  </si>
-  <si>
     <t>wm_contacts</t>
   </si>
   <si>
@@ -151,6 +148,21 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>bad_contacts</t>
+  </si>
+  <si>
+    <t>out_contacts</t>
+  </si>
+  <si>
+    <t>C'13-16</t>
+  </si>
+  <si>
+    <t>rr13-16</t>
+  </si>
+  <si>
+    <t>la10-16</t>
   </si>
 </sst>
 </file>
@@ -779,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55EA3295-E108-A141-A0DF-52F076282C70}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -796,18 +808,19 @@
     <col min="7" max="7" width="11.1640625" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.1640625" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.83203125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="47.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.33203125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="15"/>
+    <col min="10" max="10" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="18.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="6" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="7" customFormat="1" ht="102">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="102">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -815,57 +828,60 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>7</v>
+      <c r="J1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="13" customFormat="1" ht="85">
+    <row r="2" spans="1:18" s="13" customFormat="1" ht="102">
       <c r="A2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
@@ -880,49 +896,52 @@
         <v>13</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="I2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="9">
+      <c r="M2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="12"/>
+      <c r="P2" s="9">
         <v>1</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>11</v>
+      <c r="Q2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="18" customFormat="1">
+    <row r="3" spans="1:18" s="18" customFormat="1">
       <c r="A3" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="18">
         <v>4</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="18">
         <v>33</v>
@@ -931,38 +950,41 @@
         <v>25</v>
       </c>
       <c r="G3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="22"/>
+      <c r="P3" s="19">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="22"/>
-      <c r="O3" s="19">
-        <v>2</v>
-      </c>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="18" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:17" s="18" customFormat="1" ht="17">
+    <row r="4" spans="1:18" s="18" customFormat="1" ht="17">
       <c r="A4" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="18">
         <v>2</v>
@@ -977,35 +999,38 @@
         <v>10</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>31</v>
-      </c>
       <c r="K4" s="18" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="L4" s="18" t="s">
         <v>37</v>
       </c>
       <c r="M4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="22"/>
+      <c r="P4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>11</v>
+      <c r="Q4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1017,7 +1042,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1 E1:H1 C1:C3 O1:O3 I1:I3">
+  <conditionalFormatting sqref="R1 E1:H1 C1:C3 P1:P3 I1:I3">
     <cfRule type="containsBlanks" dxfId="11" priority="16">
       <formula>LEN(TRIM(C1))=0</formula>
     </cfRule>
@@ -1030,7 +1055,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2 E2:H2">
+  <conditionalFormatting sqref="R2 E2:H2">
     <cfRule type="containsBlanks" dxfId="8" priority="13">
       <formula>LEN(TRIM(E2))=0</formula>
     </cfRule>
@@ -1043,12 +1068,12 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3 E3:H3">
+  <conditionalFormatting sqref="R3 E3:H3">
     <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4 O4">
+  <conditionalFormatting sqref="C4 P4">
     <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(C4))=0</formula>
     </cfRule>
@@ -1061,7 +1086,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q4 E4:H4">
+  <conditionalFormatting sqref="R4 E4:H4">
     <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Adding updated preformatting pipeline.
</commit_message>
<xml_diff>
--- a/data/clinical_examples/test_clinicaldata.xlsx
+++ b/data/clinical_examples/test_clinicaldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam2392/Documents/eegio/data/clinical_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7DBBBF-3CD4-4E48-BCB7-314C04A94B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8435ABF0-B364-2848-93A4-C3831308EF2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{3613ACA9-70DC-9341-9578-D2DE191679B9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>patient_id</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>la10-16</t>
+  </si>
+  <si>
+    <t>resected_contacts</t>
+  </si>
+  <si>
+    <t>ablated_contacts</t>
   </si>
 </sst>
 </file>
@@ -791,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55EA3295-E108-A141-A0DF-52F076282C70}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -814,13 +820,15 @@
     <col min="13" max="13" width="47.83203125" style="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="27.33203125" style="14" customWidth="1"/>
     <col min="15" max="15" width="6" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="15"/>
+    <col min="16" max="16" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="102">
+    <row r="1" spans="1:20" s="7" customFormat="1" ht="102">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -866,17 +874,23 @@
       <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="13" customFormat="1" ht="102">
+    <row r="2" spans="1:20" s="13" customFormat="1" ht="102">
       <c r="A2" s="8" t="s">
         <v>23</v>
       </c>
@@ -920,17 +934,19 @@
         <v>14</v>
       </c>
       <c r="O2" s="12"/>
-      <c r="P2" s="9">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="9">
         <v>1</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="18" customFormat="1">
+    <row r="3" spans="1:20" s="18" customFormat="1">
       <c r="A3" s="18" t="s">
         <v>33</v>
       </c>
@@ -971,15 +987,17 @@
         <v>31</v>
       </c>
       <c r="O3" s="22"/>
-      <c r="P3" s="19">
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="19">
         <v>2</v>
       </c>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="18" t="s">
+      <c r="S3" s="19"/>
+      <c r="T3" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="18" customFormat="1" ht="17">
+    <row r="4" spans="1:20" s="18" customFormat="1" ht="17">
       <c r="A4" s="18" t="s">
         <v>34</v>
       </c>
@@ -1023,13 +1041,15 @@
         <v>31</v>
       </c>
       <c r="O4" s="22"/>
-      <c r="P4" s="19" t="s">
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="S4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="T4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1042,7 +1062,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1 E1:H1 C1:C3 P1:P3 I1:I3">
+  <conditionalFormatting sqref="T1 E1:H1 C1:C3 R1:R3 I1:I3">
     <cfRule type="containsBlanks" dxfId="11" priority="16">
       <formula>LEN(TRIM(C1))=0</formula>
     </cfRule>
@@ -1055,7 +1075,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2 E2:H2">
+  <conditionalFormatting sqref="T2 E2:H2">
     <cfRule type="containsBlanks" dxfId="8" priority="13">
       <formula>LEN(TRIM(E2))=0</formula>
     </cfRule>
@@ -1068,12 +1088,12 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3 E3:H3">
+  <conditionalFormatting sqref="T3 E3:H3">
     <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4 P4">
+  <conditionalFormatting sqref="C4 R4">
     <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(C4))=0</formula>
     </cfRule>
@@ -1086,7 +1106,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R4 E4:H4">
+  <conditionalFormatting sqref="T4 E4:H4">
     <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>

</xml_diff>